<commit_message>
Updating scoreboard based on feedback from players (round4)
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrck/Desktop/poker-tournament-leaderboard/public/res/leaderboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A9E0C4-1D86-F449-9A22-AD209DE7E384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262B319D-5366-F449-BEA7-50DB3E6C7E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="760" windowWidth="26880" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Robin</t>
+  </si>
+  <si>
+    <t>yiyang zhang</t>
+  </si>
+  <si>
+    <t>Ziqi (George) Yang</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -235,6 +241,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +548,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -593,9 +601,15 @@
       <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
       <c r="I2" s="3">
         <v>446600</v>
       </c>
@@ -616,9 +630,15 @@
       <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
       <c r="I3" s="3">
         <v>308500</v>
       </c>
@@ -639,9 +659,15 @@
       <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
       <c r="I4" s="3">
         <v>283300</v>
       </c>
@@ -662,9 +688,15 @@
       <c r="E5" s="3">
         <v>198100</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
       <c r="I5" s="3">
         <v>276100</v>
       </c>
@@ -674,68 +706,86 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3">
-        <v>224200</v>
+        <v>118500</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>139500</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3">
-        <v>224200</v>
+        <v>258000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
-        <v>1653271</v>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>224200</v>
       </c>
       <c r="D7" s="3">
-        <v>210500</v>
+        <v>0</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
       <c r="I7" s="3">
-        <v>210500</v>
+        <v>224200</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
+      <c r="B8" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>210500</v>
       </c>
       <c r="E8" s="3">
-        <v>199900</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
       <c r="I8" s="3">
-        <v>199900</v>
+        <v>210500</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -743,22 +793,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+        <v>199900</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
       <c r="I9" s="3">
-        <v>170000</v>
+        <v>199900</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -766,114 +822,144 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D10" s="3">
-        <v>152000</v>
+        <v>130000</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
       <c r="I10" s="3">
-        <v>152000</v>
+        <v>170000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>1081639</v>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>142800</v>
+        <v>152000</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
       <c r="I11" s="3">
-        <v>142800</v>
+        <v>152000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>11</v>
+      <c r="B12" s="3">
+        <v>1081639</v>
       </c>
       <c r="C12" s="3">
-        <v>121000</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>20000</v>
+        <v>142800</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
       <c r="I12" s="3">
-        <v>141000</v>
+        <v>142800</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>1357640</v>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="C13" s="3">
-        <v>135400</v>
+        <v>121000</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
       <c r="I13" s="3">
-        <v>135400</v>
+        <v>141000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
+      <c r="B14" s="3">
+        <v>1357640</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>135400</v>
       </c>
       <c r="D14" s="3">
-        <v>130700</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
       <c r="I14" s="3">
-        <v>130700</v>
+        <v>135400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -881,22 +967,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3">
         <v>0</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>130700</v>
       </c>
       <c r="E15" s="3">
-        <v>125300</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
       <c r="I15" s="3">
-        <v>125300</v>
+        <v>130700</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -904,22 +996,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C16" s="3">
-        <v>123100</v>
+        <v>0</v>
       </c>
       <c r="D16" s="3">
         <v>0</v>
       </c>
       <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+        <v>125300</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
       <c r="I16" s="3">
-        <v>123100</v>
+        <v>125300</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -927,10 +1025,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="3">
-        <v>120300</v>
+        <v>123100</v>
       </c>
       <c r="D17" s="3">
         <v>0</v>
@@ -938,11 +1036,17 @@
       <c r="E17" s="3">
         <v>0</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
       <c r="I17" s="3">
-        <v>120300</v>
+        <v>123100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -950,22 +1054,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="C18" s="3">
-        <v>0</v>
+        <v>120300</v>
       </c>
       <c r="D18" s="3">
-        <v>117800</v>
+        <v>0</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
       <c r="I18" s="3">
-        <v>117800</v>
+        <v>120300</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -973,22 +1083,28 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>117800</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
       <c r="I19" s="3">
-        <v>115700</v>
+        <v>117800</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -996,45 +1112,57 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3">
-        <v>0</v>
+        <v>115700</v>
       </c>
       <c r="D20" s="3">
-        <v>113000</v>
+        <v>0</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
       <c r="I20" s="3">
-        <v>113000</v>
+        <v>115700</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>1357925</v>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>113000</v>
       </c>
       <c r="E21" s="3">
-        <v>107500</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
       <c r="I21" s="3">
-        <v>107500</v>
+        <v>113000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1042,45 +1170,57 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>1357624</v>
+        <v>1357925</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>96400</v>
+        <v>0</v>
       </c>
       <c r="E22" s="3">
-        <v>0</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>107500</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
       <c r="I22" s="3">
-        <v>96400</v>
+        <v>107500</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>23</v>
+      <c r="B23" s="3">
+        <v>1357624</v>
       </c>
       <c r="C23" s="3">
-        <v>95600</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>96400</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
       <c r="I23" s="3">
-        <v>95600</v>
+        <v>96400</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1088,22 +1228,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <v>95600</v>
       </c>
       <c r="D24" s="3">
-        <v>91500</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
       <c r="I24" s="3">
-        <v>91500</v>
+        <v>95600</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1111,22 +1257,28 @@
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>81000</v>
+        <v>91500</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
       </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
       <c r="I25" s="3">
-        <v>81000</v>
+        <v>91500</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1134,22 +1286,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>76000</v>
+        <v>81000</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
       <c r="I26" s="3">
-        <v>76000</v>
+        <v>81000</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1157,22 +1315,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>74800</v>
+        <v>76000</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
       <c r="I27" s="3">
-        <v>74800</v>
+        <v>76000</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1180,22 +1344,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C28" s="3">
-        <v>69400</v>
+        <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>74800</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
       <c r="I28" s="3">
-        <v>69400</v>
+        <v>74800</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1203,22 +1373,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>69400</v>
       </c>
       <c r="D29" s="3">
-        <v>60400</v>
+        <v>0</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
       <c r="I29" s="3">
-        <v>60400</v>
+        <v>69400</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1226,22 +1402,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C30" s="3">
-        <v>9700</v>
+        <v>0</v>
       </c>
       <c r="D30" s="3">
-        <v>29100</v>
+        <v>60400</v>
       </c>
       <c r="E30" s="3">
-        <v>21500</v>
-      </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
       <c r="I30" s="3">
-        <v>60300</v>
+        <v>60400</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1249,68 +1431,86 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C31" s="3">
-        <v>0</v>
+        <v>9700</v>
       </c>
       <c r="D31" s="3">
-        <v>59000</v>
+        <v>29100</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+        <v>21500</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
       <c r="I31" s="3">
-        <v>59000</v>
+        <v>60300</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
-        <v>1362920</v>
+      <c r="B32" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C32" s="3">
         <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>57200</v>
+        <v>59000</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
       <c r="I32" s="3">
-        <v>57200</v>
+        <v>59000</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>40</v>
+      <c r="B33" s="3">
+        <v>1362920</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
       </c>
       <c r="D33" s="3">
-        <v>57100</v>
+        <v>57200</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
+      <c r="F33" s="3">
+        <v>0</v>
+      </c>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
       <c r="I33" s="3">
-        <v>57100</v>
+        <v>57200</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1318,22 +1518,28 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>55800</v>
+        <v>57100</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
       <c r="I34" s="3">
-        <v>55800</v>
+        <v>57100</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1341,22 +1547,28 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C35" s="3">
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>44400</v>
+        <v>55800</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="F35" s="3">
+        <v>0</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
       <c r="I35" s="3">
-        <v>44400</v>
+        <v>55800</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1364,22 +1576,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C36" s="3">
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>43000</v>
+        <v>44400</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
       <c r="I36" s="3">
-        <v>43000</v>
+        <v>44400</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1387,22 +1605,28 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="E37" s="3">
-        <v>42000</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
       <c r="I37" s="3">
-        <v>42000</v>
+        <v>43000</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -1410,68 +1634,86 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C38" s="3">
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>41400</v>
+        <v>0</v>
       </c>
       <c r="E38" s="3">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
+        <v>42000</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
       <c r="I38" s="3">
-        <v>41400</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
-        <v>1461640</v>
+      <c r="B39" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
       </c>
       <c r="D39" s="3">
-        <v>37000</v>
+        <v>41400</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
       <c r="I39" s="3">
-        <v>37000</v>
+        <v>41400</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>46</v>
+      <c r="B40" s="3">
+        <v>1461640</v>
       </c>
       <c r="C40" s="3">
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <v>36900</v>
+        <v>37000</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
       </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="F40" s="3">
+        <v>0</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
       <c r="I40" s="3">
-        <v>36900</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1479,22 +1721,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="3">
-        <v>35700</v>
+        <v>36900</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="F41" s="3">
+        <v>0</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
       <c r="I41" s="3">
-        <v>35700</v>
+        <v>36900</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1502,56 +1750,68 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C42" s="3">
         <v>0</v>
       </c>
       <c r="D42" s="3">
-        <v>32300</v>
+        <v>35700</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
       </c>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="F42" s="3">
+        <v>0</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
       <c r="I42" s="3">
-        <v>32300</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="3">
-        <v>984523</v>
+      <c r="B43" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C43" s="3">
-        <v>26000</v>
+        <v>0</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>32300</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="F43" s="3">
+        <v>0</v>
+      </c>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
       <c r="I43" s="3">
-        <v>26000</v>
+        <v>32300</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>30</v>
+      <c r="B44" s="3">
+        <v>984523</v>
       </c>
       <c r="C44" s="3">
-        <v>20000</v>
+        <v>26000</v>
       </c>
       <c r="D44" s="3">
         <v>0</v>
@@ -1559,11 +1819,17 @@
       <c r="E44" s="3">
         <v>0</v>
       </c>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
       <c r="I44" s="3">
-        <v>20000</v>
+        <v>26000</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1571,53 +1837,65 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C45" s="3">
-        <v>0</v>
+        <v>20000</v>
       </c>
       <c r="D45" s="3">
-        <v>13900</v>
+        <v>0</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="F45" s="3">
+        <v>0</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
       <c r="I45" s="3">
-        <v>13900</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
-        <v>1450367</v>
+      <c r="B46" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46" s="3">
-        <v>0</v>
+        <v>13900</v>
       </c>
       <c r="E46" s="3">
-        <v>10000</v>
-      </c>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
       <c r="I46" s="3">
-        <v>10000</v>
+        <v>13900</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>18</v>
+      <c r="B47" s="3">
+        <v>1450367</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
@@ -1626,13 +1904,19 @@
         <v>0</v>
       </c>
       <c r="E47" s="3">
-        <v>0</v>
-      </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+        <v>10000</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1640,7 +1924,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C48" s="3">
         <v>0</v>
@@ -1651,9 +1935,15 @@
       <c r="E48" s="3">
         <v>0</v>
       </c>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
       <c r="I48" s="3">
         <v>0</v>
       </c>
@@ -1663,7 +1953,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C49" s="3">
         <v>0</v>
@@ -1674,9 +1964,15 @@
       <c r="E49" s="3">
         <v>0</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
+      <c r="F49" s="3">
+        <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
       <c r="I49" s="3">
         <v>0</v>
       </c>
@@ -1686,26 +1982,58 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="3">
+        <v>0</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C50" s="3">
-        <v>0</v>
-      </c>
-      <c r="D50" s="3">
-        <v>0</v>
-      </c>
-      <c r="E50" s="3">
-        <v>0</v>
-      </c>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="2"/>
+      <c r="C51" s="5">
+        <v>0</v>
+      </c>
+      <c r="D51" s="5">
+        <v>0</v>
+      </c>
+      <c r="E51" s="5">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="2"/>
@@ -1732,8 +2060,8 @@
       <c r="A59" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I50">
-    <sortCondition descending="1" ref="I2:I50"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I51">
+    <sortCondition descending="1" ref="I2:I51"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating scoreboard round 5
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrck/Desktop/poker-tournament-leaderboard/public/res/leaderboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59494FE-1CC3-E642-9E55-0CD8D9DE8BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C261B9-6F63-694A-BAE4-D09A08BDBEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="760" windowWidth="26880" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>#</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Wiriya Kodchamitr</t>
   </si>
   <si>
-    <t>Lawrence Hider </t>
-  </si>
-  <si>
     <t>Ren En Kong </t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>Ziqi (George) Yang</t>
   </si>
   <si>
-    <t>Ameya Mahesh </t>
-  </si>
-  <si>
     <t>Patrick</t>
   </si>
   <si>
@@ -182,6 +176,9 @@
   </si>
   <si>
     <t>Ben Morrison</t>
+  </si>
+  <si>
+    <t>Jingxin Liu</t>
   </si>
 </sst>
 </file>
@@ -558,7 +555,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -614,7 +611,9 @@
       <c r="F2" s="3">
         <v>70000</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3">
         <v>516600</v>
@@ -624,50 +623,54 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>1357624</v>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>96400</v>
+        <v>283300</v>
       </c>
       <c r="E3" s="3">
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>175700</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3">
-        <v>396400</v>
+        <v>459000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>49</v>
+      <c r="B4" s="3">
+        <v>1357624</v>
       </c>
       <c r="C4" s="3">
-        <v>57400</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>96400</v>
       </c>
       <c r="E4" s="3">
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="F4" s="3">
-        <v>235800</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3">
-        <v>293200</v>
+        <v>396400</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -675,24 +678,26 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3">
-        <v>0</v>
+        <v>78000</v>
       </c>
       <c r="D5" s="3">
-        <v>283300</v>
+        <v>0</v>
       </c>
       <c r="E5" s="3">
-        <v>0</v>
+        <v>198100</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>101600</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3">
-        <v>283300</v>
+        <v>377700</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -706,18 +711,20 @@
         <v>214000</v>
       </c>
       <c r="D6" s="3">
-        <v>64500</v>
+        <v>34500</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>110700</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3">
-        <v>278500</v>
+        <v>359200</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -725,24 +732,26 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>59000</v>
+        <v>113000</v>
       </c>
       <c r="E7" s="3">
-        <v>111200</v>
+        <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>106500</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>155000</v>
+      </c>
+      <c r="G7" s="3">
+        <v>200000</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3">
-        <v>276700</v>
+        <v>355000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -750,24 +759,26 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3">
-        <v>78000</v>
+        <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>74800</v>
       </c>
       <c r="E8" s="3">
-        <v>198100</v>
+        <v>15000</v>
       </c>
       <c r="F8" s="3">
-        <v>0</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>71000</v>
+      </c>
+      <c r="G8" s="3">
+        <v>197500</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
-        <v>276100</v>
+        <v>343300</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -775,24 +786,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3">
-        <v>40000</v>
+        <v>118500</v>
       </c>
       <c r="D9" s="3">
-        <v>130000</v>
+        <v>139500</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>95500</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>75000</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3">
-        <v>265500</v>
+        <v>333000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -803,21 +816,23 @@
         <v>48</v>
       </c>
       <c r="C10" s="3">
-        <v>118500</v>
+        <v>57400</v>
       </c>
       <c r="D10" s="3">
-        <v>139500</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>235800</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3">
-        <v>258000</v>
+        <v>293200</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -825,24 +840,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>41400</v>
+        <v>55800</v>
       </c>
       <c r="E11" s="3">
-        <v>136800</v>
+        <v>130600</v>
       </c>
       <c r="F11" s="3">
-        <v>49800</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>95000</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3">
-        <v>228000</v>
+        <v>281400</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -850,49 +867,53 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3">
-        <v>224200</v>
+        <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>111200</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>106500</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3">
-        <v>224200</v>
+        <v>276700</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <v>1653271</v>
+      <c r="B13" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C13" s="3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D13" s="3">
-        <v>210500</v>
+        <v>130000</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>95500</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3">
-        <v>210500</v>
+        <v>265500</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -900,24 +921,26 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>55800</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
-        <v>130600</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>66200</v>
+      </c>
+      <c r="G14" s="3">
+        <v>193600</v>
+      </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3">
-        <v>186400</v>
+        <v>259800</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -925,49 +948,53 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>224200</v>
       </c>
       <c r="D15" s="3">
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <v>139900</v>
+        <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>45000</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3">
-        <v>184900</v>
+        <v>224200</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>39</v>
+      <c r="B16" s="3">
+        <v>1653271</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="3">
-        <v>91500</v>
+        <v>210500</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>89500</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3">
-        <v>181000</v>
+        <v>210500</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -975,24 +1002,26 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C17" s="3">
         <v>0</v>
       </c>
       <c r="D17" s="3">
-        <v>152000</v>
+        <v>0</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <v>21500</v>
-      </c>
-      <c r="G17" s="3"/>
+        <v>202000</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3">
-        <v>173500</v>
+        <v>202000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1000,24 +1029,26 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>41400</v>
       </c>
       <c r="E18" s="3">
-        <v>0</v>
+        <v>136800</v>
       </c>
       <c r="F18" s="3">
-        <v>157500</v>
-      </c>
-      <c r="G18" s="3"/>
+        <v>19800</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3">
-        <v>157500</v>
+        <v>198000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1025,24 +1056,26 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="C19" s="3">
-        <v>0</v>
+        <v>121000</v>
       </c>
       <c r="D19" s="3">
-        <v>113000</v>
+        <v>20000</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>155000</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>51000</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3">
-        <v>155000</v>
+        <v>192000</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1050,49 +1083,53 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>43000</v>
+        <v>0</v>
       </c>
       <c r="E20" s="3">
-        <v>72200</v>
+        <v>139900</v>
       </c>
       <c r="F20" s="3">
-        <v>32600</v>
-      </c>
-      <c r="G20" s="3"/>
+        <v>45000</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3">
-        <v>147800</v>
+        <v>184900</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>1081639</v>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>142800</v>
+        <v>91500</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
       </c>
       <c r="F21" s="3">
-        <v>0</v>
-      </c>
-      <c r="G21" s="3"/>
+        <v>89500</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3">
-        <v>142800</v>
+        <v>181000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1100,63 +1137,67 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="C22" s="3">
-        <v>121000</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>20000</v>
+        <v>30400</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>0</v>
-      </c>
-      <c r="G22" s="3"/>
+        <v>140000</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3">
-        <v>141000</v>
+        <v>170400</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>1357640</v>
+      <c r="B23" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C23" s="3">
-        <v>135400</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>72200</v>
       </c>
       <c r="F23" s="3">
-        <v>0</v>
-      </c>
-      <c r="G23" s="3"/>
+        <v>32600</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3">
-        <v>135400</v>
+        <v>147800</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>25</v>
+      <c r="B24" s="3">
+        <v>1081639</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>130700</v>
+        <v>142800</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -1164,35 +1205,39 @@
       <c r="F24" s="3">
         <v>0</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3">
-        <v>130700</v>
+        <v>142800</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>43</v>
+      <c r="B25" s="3">
+        <v>1357640</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <v>135400</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
       </c>
       <c r="E25" s="3">
-        <v>125300</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3">
         <v>0</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="I25" s="3">
-        <v>125300</v>
+        <v>135400</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1200,13 +1245,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C26" s="3">
-        <v>123100</v>
+        <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>130700</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -1214,35 +1259,39 @@
       <c r="F26" s="3">
         <v>0</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
-        <v>123100</v>
+        <v>130700</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
-        <v>1362920</v>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C27" s="3">
         <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>57200</v>
+        <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>125300</v>
       </c>
       <c r="F27" s="3">
-        <v>65000</v>
-      </c>
-      <c r="G27" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3">
-        <v>122200</v>
+        <v>125300</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1250,10 +1299,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C28" s="3">
-        <v>120300</v>
+        <v>123100</v>
       </c>
       <c r="D28" s="3">
         <v>0</v>
@@ -1264,35 +1313,39 @@
       <c r="F28" s="3">
         <v>0</v>
       </c>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <v>0</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
-        <v>120300</v>
+        <v>123100</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>35</v>
+      <c r="B29" s="3">
+        <v>1362920</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
       </c>
       <c r="D29" s="3">
-        <v>117800</v>
+        <v>57200</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="3"/>
+        <v>65000</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
-        <v>117800</v>
+        <v>122200</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1300,10 +1353,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="3">
-        <v>115700</v>
+        <v>120300</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
@@ -1314,35 +1367,39 @@
       <c r="F30" s="3">
         <v>0</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3">
+        <v>0</v>
+      </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
-        <v>115700</v>
+        <v>120300</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
-        <v>1357925</v>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C31" s="3">
         <v>0</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
+        <v>117800</v>
       </c>
       <c r="E31" s="3">
-        <v>107500</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3">
         <v>0</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3">
+        <v>0</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
-        <v>107500</v>
+        <v>117800</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1350,49 +1407,53 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C32" s="3">
-        <v>0</v>
+        <v>115700</v>
       </c>
       <c r="D32" s="3">
         <v>0</v>
       </c>
       <c r="E32" s="3">
-        <v>102400</v>
+        <v>0</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
-        <v>102400</v>
+        <v>115700</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>23</v>
+      <c r="B33" s="3">
+        <v>1357925</v>
       </c>
       <c r="C33" s="3">
-        <v>95600</v>
+        <v>0</v>
       </c>
       <c r="D33" s="3">
         <v>0</v>
       </c>
       <c r="E33" s="3">
-        <v>0</v>
+        <v>107500</v>
       </c>
       <c r="F33" s="3">
         <v>0</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
-        <v>95600</v>
+        <v>107500</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -1400,24 +1461,26 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>74800</v>
+        <v>0</v>
       </c>
       <c r="E34" s="3">
-        <v>15000</v>
+        <v>102400</v>
       </c>
       <c r="F34" s="3">
         <v>0</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
-        <v>89800</v>
+        <v>102400</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1425,13 +1488,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C35" s="3">
-        <v>0</v>
+        <v>95600</v>
       </c>
       <c r="D35" s="3">
-        <v>81000</v>
+        <v>0</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
@@ -1439,10 +1502,12 @@
       <c r="F35" s="3">
         <v>0</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
-        <v>81000</v>
+        <v>95600</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1450,24 +1515,26 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="C36" s="3">
-        <v>0</v>
+        <v>9700</v>
       </c>
       <c r="D36" s="3">
-        <v>0</v>
+        <v>29100</v>
       </c>
       <c r="E36" s="3">
-        <v>0</v>
+        <v>21500</v>
       </c>
       <c r="F36" s="3">
-        <v>79400</v>
-      </c>
-      <c r="G36" s="3"/>
+        <v>42100</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
-        <v>79400</v>
+        <v>92700</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1475,24 +1542,26 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C37" s="3">
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>76000</v>
+        <v>0</v>
       </c>
       <c r="E37" s="3">
-        <v>0</v>
+        <v>81500</v>
       </c>
       <c r="F37" s="3">
         <v>0</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
-        <v>76000</v>
+        <v>81500</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
@@ -1500,13 +1569,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="C38" s="3">
-        <v>69400</v>
+        <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>0</v>
+        <v>81000</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
@@ -1514,10 +1583,12 @@
       <c r="F38" s="3">
         <v>0</v>
       </c>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3">
-        <v>69400</v>
+        <v>81000</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -1525,7 +1596,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C39" s="3">
         <v>0</v>
@@ -1537,12 +1608,14 @@
         <v>0</v>
       </c>
       <c r="F39" s="3">
-        <v>66200</v>
-      </c>
-      <c r="G39" s="3"/>
+        <v>79400</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3">
-        <v>66200</v>
+        <v>79400</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -1550,24 +1623,26 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="C40" s="3">
-        <v>9700</v>
+        <v>0</v>
       </c>
       <c r="D40" s="3">
-        <v>29100</v>
+        <v>0</v>
       </c>
       <c r="E40" s="3">
-        <v>21500</v>
+        <v>0</v>
       </c>
       <c r="F40" s="3">
         <v>0</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3">
+        <v>78900</v>
+      </c>
       <c r="H40" s="3"/>
       <c r="I40" s="3">
-        <v>60300</v>
+        <v>78900</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1575,13 +1650,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C41" s="3">
         <v>0</v>
       </c>
       <c r="D41" s="3">
-        <v>57100</v>
+        <v>76000</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -1589,10 +1664,12 @@
       <c r="F41" s="3">
         <v>0</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3">
+        <v>0</v>
+      </c>
       <c r="H41" s="3"/>
       <c r="I41" s="3">
-        <v>57100</v>
+        <v>76000</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1600,13 +1677,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C42" s="3">
-        <v>0</v>
+        <v>69400</v>
       </c>
       <c r="D42" s="3">
-        <v>44400</v>
+        <v>0</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -1614,10 +1691,12 @@
       <c r="F42" s="3">
         <v>0</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
-        <v>44400</v>
+        <v>69400</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1625,38 +1704,40 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C43" s="3">
         <v>0</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>57100</v>
       </c>
       <c r="E43" s="3">
-        <v>42000</v>
+        <v>0</v>
       </c>
       <c r="F43" s="3">
         <v>0</v>
       </c>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3">
+        <v>0</v>
+      </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3">
-        <v>42000</v>
+        <v>57100</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
-      <c r="B44" s="3">
-        <v>1461640</v>
+      <c r="B44" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>37000</v>
+        <v>44400</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
@@ -1664,10 +1745,12 @@
       <c r="F44" s="3">
         <v>0</v>
       </c>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3">
-        <v>37000</v>
+        <v>44400</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -1675,38 +1758,40 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
       </c>
       <c r="D45" s="3">
-        <v>36900</v>
+        <v>0</v>
       </c>
       <c r="E45" s="3">
-        <v>0</v>
+        <v>42000</v>
       </c>
       <c r="F45" s="3">
         <v>0</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3">
+        <v>0</v>
+      </c>
       <c r="H45" s="3"/>
       <c r="I45" s="3">
-        <v>36900</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>42</v>
+      <c r="B46" s="3">
+        <v>1461640</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46" s="3">
-        <v>35700</v>
+        <v>37000</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
@@ -1714,10 +1799,12 @@
       <c r="F46" s="3">
         <v>0</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
       <c r="H46" s="3"/>
       <c r="I46" s="3">
-        <v>35700</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1725,13 +1812,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>32300</v>
+        <v>35700</v>
       </c>
       <c r="E47" s="3">
         <v>0</v>
@@ -1739,10 +1826,12 @@
       <c r="F47" s="3">
         <v>0</v>
       </c>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3">
+        <v>0</v>
+      </c>
       <c r="H47" s="3"/>
       <c r="I47" s="3">
-        <v>32300</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1750,13 +1839,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C48" s="3">
         <v>0</v>
       </c>
       <c r="D48" s="3">
-        <v>30400</v>
+        <v>32300</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
@@ -1764,10 +1853,12 @@
       <c r="F48" s="3">
         <v>0</v>
       </c>
-      <c r="G48" s="3"/>
+      <c r="G48" s="3">
+        <v>0</v>
+      </c>
       <c r="H48" s="3"/>
       <c r="I48" s="3">
-        <v>30400</v>
+        <v>32300</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1789,7 +1880,9 @@
       <c r="F49" s="3">
         <v>0</v>
       </c>
-      <c r="G49" s="3"/>
+      <c r="G49" s="3">
+        <v>0</v>
+      </c>
       <c r="H49" s="3"/>
       <c r="I49" s="3">
         <v>26000</v>
@@ -1814,7 +1907,9 @@
       <c r="F50" s="3">
         <v>0</v>
       </c>
-      <c r="G50" s="3"/>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3">
         <v>20000</v>
@@ -1839,7 +1934,9 @@
       <c r="F51" s="3">
         <v>0</v>
       </c>
-      <c r="G51" s="3"/>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3">
         <v>13900</v>
@@ -1864,7 +1961,9 @@
       <c r="F52" s="3">
         <v>0</v>
       </c>
-      <c r="G52" s="3"/>
+      <c r="G52" s="3">
+        <v>0</v>
+      </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3">
         <v>10000</v>
@@ -1875,13 +1974,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="C53" s="3">
         <v>0</v>
       </c>
       <c r="D53" s="3">
-        <v>0</v>
+        <v>6900</v>
       </c>
       <c r="E53" s="3">
         <v>0</v>
@@ -1889,10 +1988,12 @@
       <c r="F53" s="3">
         <v>0</v>
       </c>
-      <c r="G53" s="3"/>
+      <c r="G53" s="3">
+        <v>0</v>
+      </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3">
-        <v>0</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -1914,7 +2015,9 @@
       <c r="F54" s="3">
         <v>0</v>
       </c>
-      <c r="G54" s="3"/>
+      <c r="G54" s="3">
+        <v>0</v>
+      </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3">
         <v>0</v>
@@ -1925,7 +2028,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C55" s="3">
         <v>0</v>
@@ -1939,7 +2042,9 @@
       <c r="F55" s="3">
         <v>0</v>
       </c>
-      <c r="G55" s="3"/>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
       <c r="H55" s="3"/>
       <c r="I55" s="3">
         <v>0</v>
@@ -1949,8 +2054,8 @@
       <c r="A56" s="1">
         <v>55</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>51</v>
+      <c r="B56" s="3">
+        <v>1464487</v>
       </c>
       <c r="C56" s="3">
         <v>0</v>
@@ -1964,36 +2069,24 @@
       <c r="F56" s="3">
         <v>0</v>
       </c>
-      <c r="G56" s="3"/>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
-        <v>56</v>
-      </c>
-      <c r="B57" s="3">
-        <v>1464487</v>
-      </c>
-      <c r="C57" s="3">
-        <v>0</v>
-      </c>
-      <c r="D57" s="3">
-        <v>0</v>
-      </c>
-      <c r="E57" s="3">
-        <v>0</v>
-      </c>
-      <c r="F57" s="3">
-        <v>0</v>
-      </c>
+      <c r="A57" s="2"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="3">
-        <v>0</v>
-      </c>
+      <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="2"/>
@@ -2002,8 +2095,8 @@
       <c r="A59" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I57">
-    <sortCondition descending="1" ref="I2:I57"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I56">
+    <sortCondition descending="1" ref="I2:I56"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating scoreboard round 6 FINAL ROUND
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrck/Desktop/poker-tournament-leaderboard/public/res/leaderboards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C261B9-6F63-694A-BAE4-D09A08BDBEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9505B74-5CF5-DA42-836F-31C196CC38C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="760" windowWidth="26880" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Jingxin Liu</t>
+  </si>
+  <si>
+    <t>Hanryk Li</t>
   </si>
 </sst>
 </file>
@@ -555,7 +558,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -597,26 +600,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C2" s="3">
-        <v>294300</v>
+        <v>57400</v>
       </c>
       <c r="D2" s="3">
-        <v>152300</v>
+        <v>0</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
       </c>
       <c r="F2" s="3">
-        <v>70000</v>
+        <v>235800</v>
       </c>
       <c r="G2" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="3"/>
+      <c r="H2" s="3">
+        <v>289400</v>
+      </c>
       <c r="I2" s="3">
-        <v>516600</v>
+        <v>582600</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -624,26 +629,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>294300</v>
       </c>
       <c r="D3" s="3">
-        <v>283300</v>
+        <v>152300</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
       </c>
       <c r="F3" s="3">
-        <v>175700</v>
+        <v>70000</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
       <c r="I3" s="3">
-        <v>459000</v>
+        <v>516600</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -666,11 +673,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3"/>
+        <v>99400</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
       <c r="I4" s="3">
-        <v>396400</v>
+        <v>495800</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -678,26 +687,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C5" s="3">
-        <v>78000</v>
+        <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>283300</v>
       </c>
       <c r="E5" s="3">
-        <v>198100</v>
+        <v>0</v>
       </c>
       <c r="F5" s="3">
-        <v>0</v>
+        <v>145700</v>
       </c>
       <c r="G5" s="3">
-        <v>101600</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>62400</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
       <c r="I5" s="3">
-        <v>377700</v>
+        <v>491400</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -705,26 +716,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3">
-        <v>214000</v>
+        <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>34500</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>110700</v>
+        <v>202000</v>
       </c>
       <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>230000</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3">
-        <v>359200</v>
+        <v>432000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -732,26 +745,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C7" s="3">
-        <v>0</v>
+        <v>184000</v>
       </c>
       <c r="D7" s="3">
-        <v>113000</v>
+        <v>64500</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
       </c>
       <c r="F7" s="3">
-        <v>155000</v>
+        <v>110700</v>
       </c>
       <c r="G7" s="3">
-        <v>200000</v>
-      </c>
-      <c r="H7" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>128000</v>
+      </c>
       <c r="I7" s="3">
-        <v>355000</v>
+        <v>422700</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -759,26 +774,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>118500</v>
       </c>
       <c r="D8" s="3">
-        <v>74800</v>
+        <v>139500</v>
       </c>
       <c r="E8" s="3">
-        <v>15000</v>
+        <v>0</v>
       </c>
       <c r="F8" s="3">
-        <v>71000</v>
+        <v>75000</v>
       </c>
       <c r="G8" s="3">
-        <v>197500</v>
-      </c>
-      <c r="H8" s="3"/>
+        <v>151100</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
       <c r="I8" s="3">
-        <v>343300</v>
+        <v>409100</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -786,26 +803,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C9" s="3">
-        <v>118500</v>
+        <v>40000</v>
       </c>
       <c r="D9" s="3">
-        <v>139500</v>
+        <v>130000</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
       </c>
       <c r="F9" s="3">
-        <v>75000</v>
+        <v>95500</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
       </c>
-      <c r="H9" s="3"/>
+      <c r="H9" s="3">
+        <v>159800</v>
+      </c>
       <c r="I9" s="3">
-        <v>333000</v>
+        <v>385300</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -813,26 +832,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C10" s="3">
-        <v>57400</v>
+        <v>78000</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <v>0</v>
+        <v>198100</v>
       </c>
       <c r="F10" s="3">
-        <v>235800</v>
+        <v>0</v>
       </c>
       <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3"/>
+        <v>101600</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
       <c r="I10" s="3">
-        <v>293200</v>
+        <v>377700</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -840,26 +861,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>55800</v>
+        <v>74800</v>
       </c>
       <c r="E11" s="3">
-        <v>130600</v>
+        <v>15000</v>
       </c>
       <c r="F11" s="3">
-        <v>95000</v>
+        <v>71000</v>
       </c>
       <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3"/>
+        <v>197500</v>
+      </c>
+      <c r="H11" s="3">
+        <v>104500</v>
+      </c>
       <c r="I11" s="3">
-        <v>281400</v>
+        <v>376800</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -884,9 +907,11 @@
       <c r="G12" s="3">
         <v>0</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="H12" s="3">
+        <v>152100</v>
+      </c>
       <c r="I12" s="3">
-        <v>276700</v>
+        <v>369800</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -894,26 +919,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D13" s="3">
-        <v>130000</v>
+        <v>0</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
       </c>
       <c r="F13" s="3">
-        <v>95500</v>
+        <v>66200</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3"/>
+        <v>193600</v>
+      </c>
+      <c r="H13" s="3">
+        <v>102900</v>
+      </c>
       <c r="I13" s="3">
-        <v>265500</v>
+        <v>362700</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -921,26 +948,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>55800</v>
       </c>
       <c r="E14" s="3">
-        <v>0</v>
+        <v>130600</v>
       </c>
       <c r="F14" s="3">
-        <v>66200</v>
+        <v>0</v>
       </c>
       <c r="G14" s="3">
-        <v>193600</v>
-      </c>
-      <c r="H14" s="3"/>
+        <v>175000</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
       <c r="I14" s="3">
-        <v>259800</v>
+        <v>361400</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -948,26 +977,28 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3">
-        <v>224200</v>
+        <v>0</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>113000</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <v>155000</v>
       </c>
       <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3"/>
+        <v>200000</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
       <c r="I15" s="3">
-        <v>224200</v>
+        <v>355000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -975,26 +1006,28 @@
         <v>15</v>
       </c>
       <c r="B16" s="3">
-        <v>1653271</v>
+        <v>1081639</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
       </c>
       <c r="D16" s="3">
-        <v>210500</v>
+        <v>142800</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
       <c r="F16" s="3">
-        <v>0</v>
+        <v>175700</v>
       </c>
       <c r="G16" s="3">
         <v>0</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
       <c r="I16" s="3">
-        <v>210500</v>
+        <v>318500</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
@@ -1002,26 +1035,28 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3">
-        <v>0</v>
+        <v>135400</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>91500</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
       </c>
       <c r="F17" s="3">
-        <v>202000</v>
+        <v>89500</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
       <c r="I17" s="3">
-        <v>202000</v>
+        <v>316400</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1029,26 +1064,28 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3">
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>41400</v>
+        <v>0</v>
       </c>
       <c r="E18" s="3">
-        <v>136800</v>
+        <v>139900</v>
       </c>
       <c r="F18" s="3">
-        <v>19800</v>
+        <v>45000</v>
       </c>
       <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3"/>
+        <v>105000</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
       <c r="I18" s="3">
-        <v>198000</v>
+        <v>289900</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1056,53 +1093,57 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3">
-        <v>121000</v>
+        <v>224200</v>
       </c>
       <c r="D19" s="3">
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>51000</v>
+        <v>0</v>
       </c>
       <c r="G19" s="3">
         <v>0</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
       <c r="I19" s="3">
-        <v>192000</v>
+        <v>224200</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+      <c r="B20" s="3">
+        <v>1653271</v>
       </c>
       <c r="C20" s="3">
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>210500</v>
       </c>
       <c r="E20" s="3">
-        <v>139900</v>
+        <v>0</v>
       </c>
       <c r="F20" s="3">
-        <v>45000</v>
+        <v>0</v>
       </c>
       <c r="G20" s="3">
         <v>0</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
       <c r="I20" s="3">
-        <v>184900</v>
+        <v>210500</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1110,26 +1151,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C21" s="3">
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>91500</v>
+        <v>41400</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>136800</v>
       </c>
       <c r="F21" s="3">
-        <v>89500</v>
+        <v>19800</v>
       </c>
       <c r="G21" s="3">
         <v>0</v>
       </c>
-      <c r="H21" s="3"/>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
       <c r="I21" s="3">
-        <v>181000</v>
+        <v>198000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1137,26 +1180,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C22" s="3">
-        <v>0</v>
+        <v>121000</v>
       </c>
       <c r="D22" s="3">
-        <v>30400</v>
+        <v>20000</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>140000</v>
+        <v>51000</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
       </c>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
       <c r="I22" s="3">
-        <v>170400</v>
+        <v>192000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1164,67 +1209,71 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C23" s="3">
         <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>43000</v>
+        <v>44400</v>
       </c>
       <c r="E23" s="3">
-        <v>72200</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>32600</v>
+        <v>140000</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
       <c r="I23" s="3">
-        <v>147800</v>
+        <v>184400</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
-        <v>1081639</v>
+      <c r="B24" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>142800</v>
+        <v>43000</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>72200</v>
       </c>
       <c r="F24" s="3">
-        <v>0</v>
+        <v>32600</v>
       </c>
       <c r="G24" s="3">
         <v>0</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
       <c r="I24" s="3">
-        <v>142800</v>
+        <v>147800</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
-        <v>1357640</v>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="C25" s="3">
-        <v>135400</v>
+        <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>0</v>
+        <v>130700</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -1235,9 +1284,11 @@
       <c r="G25" s="3">
         <v>0</v>
       </c>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
       <c r="I25" s="3">
-        <v>135400</v>
+        <v>130700</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1245,16 +1296,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>130700</v>
+        <v>0</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>125300</v>
       </c>
       <c r="F26" s="3">
         <v>0</v>
@@ -1262,9 +1313,11 @@
       <c r="G26" s="3">
         <v>0</v>
       </c>
-      <c r="H26" s="3"/>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
       <c r="I26" s="3">
-        <v>130700</v>
+        <v>125300</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1272,16 +1325,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <v>123100</v>
       </c>
       <c r="D27" s="3">
         <v>0</v>
       </c>
       <c r="E27" s="3">
-        <v>125300</v>
+        <v>0</v>
       </c>
       <c r="F27" s="3">
         <v>0</v>
@@ -1289,63 +1342,69 @@
       <c r="G27" s="3">
         <v>0</v>
       </c>
-      <c r="H27" s="3"/>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
       <c r="I27" s="3">
-        <v>125300</v>
+        <v>123100</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>16</v>
+      <c r="B28" s="3">
+        <v>1362920</v>
       </c>
       <c r="C28" s="3">
-        <v>123100</v>
+        <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>57200</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
       </c>
       <c r="F28" s="3">
-        <v>0</v>
+        <v>65000</v>
       </c>
       <c r="G28" s="3">
         <v>0</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
       <c r="I28" s="3">
-        <v>123100</v>
+        <v>122200</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
-        <v>1362920</v>
+      <c r="B29" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C29" s="3">
-        <v>0</v>
+        <v>120300</v>
       </c>
       <c r="D29" s="3">
-        <v>57200</v>
+        <v>0</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
       </c>
       <c r="F29" s="3">
-        <v>65000</v>
+        <v>0</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
       </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
       <c r="I29" s="3">
-        <v>122200</v>
+        <v>120300</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1353,26 +1412,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C30" s="3">
-        <v>120300</v>
+        <v>9700</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>29100</v>
       </c>
       <c r="E30" s="3">
-        <v>0</v>
+        <v>21500</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>42100</v>
       </c>
       <c r="G30" s="3">
-        <v>0</v>
-      </c>
-      <c r="H30" s="3"/>
+        <v>48800</v>
+      </c>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
       <c r="I30" s="3">
-        <v>120300</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
@@ -1397,7 +1458,9 @@
       <c r="G31" s="3">
         <v>0</v>
       </c>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
       <c r="I31" s="3">
         <v>117800</v>
       </c>
@@ -1424,7 +1487,9 @@
       <c r="G32" s="3">
         <v>0</v>
       </c>
-      <c r="H32" s="3"/>
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
       <c r="I32" s="3">
         <v>115700</v>
       </c>
@@ -1433,8 +1498,8 @@
       <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>1357925</v>
+      <c r="B33" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="C33" s="3">
         <v>0</v>
@@ -1443,25 +1508,27 @@
         <v>0</v>
       </c>
       <c r="E33" s="3">
-        <v>107500</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3">
-        <v>0</v>
+        <v>109300</v>
       </c>
       <c r="G33" s="3">
         <v>0</v>
       </c>
-      <c r="H33" s="3"/>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
       <c r="I33" s="3">
-        <v>107500</v>
+        <v>109300</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>50</v>
+      <c r="B34" s="3">
+        <v>1357925</v>
       </c>
       <c r="C34" s="3">
         <v>0</v>
@@ -1470,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="3">
-        <v>102400</v>
+        <v>107500</v>
       </c>
       <c r="F34" s="3">
         <v>0</v>
@@ -1478,9 +1545,11 @@
       <c r="G34" s="3">
         <v>0</v>
       </c>
-      <c r="H34" s="3"/>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
       <c r="I34" s="3">
-        <v>102400</v>
+        <v>107500</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -1488,16 +1557,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C35" s="3">
-        <v>95600</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3">
         <v>0</v>
       </c>
       <c r="E35" s="3">
-        <v>0</v>
+        <v>102400</v>
       </c>
       <c r="F35" s="3">
         <v>0</v>
@@ -1505,9 +1574,11 @@
       <c r="G35" s="3">
         <v>0</v>
       </c>
-      <c r="H35" s="3"/>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
       <c r="I35" s="3">
-        <v>95600</v>
+        <v>102400</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1515,26 +1586,28 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C36" s="3">
-        <v>9700</v>
+        <v>95600</v>
       </c>
       <c r="D36" s="3">
-        <v>29100</v>
+        <v>0</v>
       </c>
       <c r="E36" s="3">
-        <v>21500</v>
+        <v>0</v>
       </c>
       <c r="F36" s="3">
-        <v>42100</v>
+        <v>0</v>
       </c>
       <c r="G36" s="3">
         <v>0</v>
       </c>
-      <c r="H36" s="3"/>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
       <c r="I36" s="3">
-        <v>92700</v>
+        <v>95600</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -1559,7 +1632,9 @@
       <c r="G37" s="3">
         <v>0</v>
       </c>
-      <c r="H37" s="3"/>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
       <c r="I37" s="3">
         <v>81500</v>
       </c>
@@ -1586,7 +1661,9 @@
       <c r="G38" s="3">
         <v>0</v>
       </c>
-      <c r="H38" s="3"/>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
       <c r="I38" s="3">
         <v>81000</v>
       </c>
@@ -1613,7 +1690,9 @@
       <c r="G39" s="3">
         <v>0</v>
       </c>
-      <c r="H39" s="3"/>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
       <c r="I39" s="3">
         <v>79400</v>
       </c>
@@ -1640,7 +1719,9 @@
       <c r="G40" s="3">
         <v>78900</v>
       </c>
-      <c r="H40" s="3"/>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
       <c r="I40" s="3">
         <v>78900</v>
       </c>
@@ -1667,7 +1748,9 @@
       <c r="G41" s="3">
         <v>0</v>
       </c>
-      <c r="H41" s="3"/>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
       <c r="I41" s="3">
         <v>76000</v>
       </c>
@@ -1694,7 +1777,9 @@
       <c r="G42" s="3">
         <v>0</v>
       </c>
-      <c r="H42" s="3"/>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
       <c r="I42" s="3">
         <v>69400</v>
       </c>
@@ -1721,7 +1806,9 @@
       <c r="G43" s="3">
         <v>0</v>
       </c>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
       <c r="I43" s="3">
         <v>57100</v>
       </c>
@@ -1731,16 +1818,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C44" s="3">
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>44400</v>
+        <v>0</v>
       </c>
       <c r="E44" s="3">
-        <v>0</v>
+        <v>42000</v>
       </c>
       <c r="F44" s="3">
         <v>0</v>
@@ -1748,26 +1835,28 @@
       <c r="G44" s="3">
         <v>0</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
       <c r="I44" s="3">
-        <v>44400</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>44</v>
+      <c r="B45" s="3">
+        <v>1461640</v>
       </c>
       <c r="C45" s="3">
         <v>0</v>
       </c>
       <c r="D45" s="3">
-        <v>0</v>
+        <v>37000</v>
       </c>
       <c r="E45" s="3">
-        <v>42000</v>
+        <v>0</v>
       </c>
       <c r="F45" s="3">
         <v>0</v>
@@ -1775,23 +1864,25 @@
       <c r="G45" s="3">
         <v>0</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
       <c r="I45" s="3">
-        <v>42000</v>
+        <v>37000</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
-        <v>1461640</v>
+      <c r="B46" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C46" s="3">
         <v>0</v>
       </c>
       <c r="D46" s="3">
-        <v>37000</v>
+        <v>35700</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
@@ -1802,9 +1893,11 @@
       <c r="G46" s="3">
         <v>0</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
       <c r="I46" s="3">
-        <v>37000</v>
+        <v>35700</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1812,13 +1905,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C47" s="3">
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>35700</v>
+        <v>32300</v>
       </c>
       <c r="E47" s="3">
         <v>0</v>
@@ -1829,9 +1922,11 @@
       <c r="G47" s="3">
         <v>0</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
       <c r="I47" s="3">
-        <v>35700</v>
+        <v>32300</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1839,13 +1934,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C48" s="3">
         <v>0</v>
       </c>
       <c r="D48" s="3">
-        <v>32300</v>
+        <v>30400</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
@@ -1856,9 +1951,11 @@
       <c r="G48" s="3">
         <v>0</v>
       </c>
-      <c r="H48" s="3"/>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
       <c r="I48" s="3">
-        <v>32300</v>
+        <v>30400</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
@@ -1883,7 +1980,9 @@
       <c r="G49" s="3">
         <v>0</v>
       </c>
-      <c r="H49" s="3"/>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
       <c r="I49" s="3">
         <v>26000</v>
       </c>
@@ -1910,7 +2009,9 @@
       <c r="G50" s="3">
         <v>0</v>
       </c>
-      <c r="H50" s="3"/>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
       <c r="I50" s="3">
         <v>20000</v>
       </c>
@@ -1937,7 +2038,9 @@
       <c r="G51" s="3">
         <v>0</v>
       </c>
-      <c r="H51" s="3"/>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
       <c r="I51" s="3">
         <v>13900</v>
       </c>
@@ -1964,7 +2067,9 @@
       <c r="G52" s="3">
         <v>0</v>
       </c>
-      <c r="H52" s="3"/>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
       <c r="I52" s="3">
         <v>10000</v>
       </c>
@@ -1991,7 +2096,9 @@
       <c r="G53" s="3">
         <v>0</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
       <c r="I53" s="3">
         <v>6900</v>
       </c>
@@ -2001,7 +2108,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C54" s="3">
         <v>0</v>
@@ -2018,7 +2125,9 @@
       <c r="G54" s="3">
         <v>0</v>
       </c>
-      <c r="H54" s="3"/>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
       <c r="I54" s="3">
         <v>0</v>
       </c>
@@ -2028,7 +2137,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="C55" s="3">
         <v>0</v>
@@ -2045,7 +2154,9 @@
       <c r="G55" s="3">
         <v>0</v>
       </c>
-      <c r="H55" s="3"/>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
       <c r="I55" s="3">
         <v>0</v>
       </c>
@@ -2072,7 +2183,9 @@
       <c r="G56" s="3">
         <v>0</v>
       </c>
-      <c r="H56" s="3"/>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
       <c r="I56" s="3">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated leaderboards for round2
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Downloads\Chrome Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41521E65-7AE8-406F-A7D6-010237F98E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15CFF69-2ABB-498C-9286-5F7C191C4A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1990" yWindow="4580" windowWidth="19060" windowHeight="10270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="8520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -62,14 +62,56 @@
     <t>Total</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Chenul Punchihewa</t>
+  </si>
+  <si>
+    <t>Phan Minh Quan Nguyen</t>
+  </si>
+  <si>
+    <t>Haopen Jiang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ho Chon Wang </t>
+  </si>
+  <si>
+    <t>Minh Hoang Ha</t>
+  </si>
+  <si>
+    <t>Marcus Gan</t>
+  </si>
+  <si>
+    <t>Yige Tan</t>
+  </si>
+  <si>
+    <t>Shilong Wan</t>
+  </si>
+  <si>
+    <t>Yan Hei Hui</t>
+  </si>
+  <si>
+    <t>Benjamin Morrison</t>
+  </si>
+  <si>
+    <t>Zarif Syed</t>
+  </si>
+  <si>
+    <t>Zac Zhang</t>
+  </si>
+  <si>
+    <t>Long Ha</t>
+  </si>
+  <si>
+    <t>Liyao Ren</t>
+  </si>
+  <si>
+    <t>Max Guo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +129,20 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -112,10 +168,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,15 +476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="27.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -462,523 +520,469 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
+      <c r="C2" s="3">
+        <v>169400</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>169400</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3">
+        <v>140000</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>140000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>136000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>136000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>126900</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>126900</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <v>0</v>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>100900</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>100900</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0</v>
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>96200</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>96200</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>81600</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>81600</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="3">
+        <v>75000</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>75000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3">
+        <v>69300</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>69300</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
+      <c r="B11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>66400</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>66400</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3">
+        <v>62800</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>62800</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
+      <c r="B13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3">
+        <v>62000</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>62000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
+      <c r="B14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3">
+        <v>55000</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>55000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
+      <c r="B15" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3">
+        <v>49400</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>49400</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>28000</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>28000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
@@ -2168,42 +2172,9 @@
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A130" s="2"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-      <c r="F130" s="1"/>
-      <c r="G130" s="1"/>
-      <c r="H130" s="1"/>
-      <c r="I130" s="1"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A131" s="2"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1"/>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
-      <c r="F131" s="1"/>
-      <c r="G131" s="1"/>
-      <c r="H131" s="1"/>
-      <c r="I131" s="1"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A132" s="2"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
-      <c r="D132" s="1"/>
-      <c r="E132" s="1"/>
-      <c r="F132" s="1"/>
-      <c r="G132" s="1"/>
-      <c r="H132" s="1"/>
-      <c r="I132" s="1"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I112">
-    <sortCondition descending="1" ref="I2:I112"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I109">
+    <sortCondition descending="1" ref="I2:I109"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
updated for round 3
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Downloads\Chrome Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12DC45D-F857-4D85-B0CA-DC96C396050A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC227B-ECFF-4042-8EA1-28CA7D613256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Haopen Jiang</t>
   </si>
   <si>
-    <t xml:space="preserve">Ho Chon Wang </t>
-  </si>
-  <si>
     <t>Minh Hoang Ha</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>Edwin Zou</t>
   </si>
   <si>
-    <t>JAY TIMOTHY WANG</t>
-  </si>
-  <si>
     <t>Hanhan Chen</t>
   </si>
   <si>
@@ -129,6 +123,30 @@
   </si>
   <si>
     <t>Gabriel Lorenzo Geronimo</t>
+  </si>
+  <si>
+    <t>Ho Chon Wang</t>
+  </si>
+  <si>
+    <t>Jay Timothy Wang</t>
+  </si>
+  <si>
+    <t>Mohit Garg</t>
+  </si>
+  <si>
+    <t>Darius Goh</t>
+  </si>
+  <si>
+    <t>Yuhao Guo</t>
+  </si>
+  <si>
+    <t>Hugh Roberts</t>
+  </si>
+  <si>
+    <t>Gordon Wu</t>
+  </si>
+  <si>
+    <t>Bervyn Sim</t>
   </si>
 </sst>
 </file>
@@ -172,10 +190,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,14 +498,13 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="2"/>
-    <col min="2" max="2" width="27.08984375" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="2"/>
+    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -524,28 +540,28 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>387500</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <v>387500</v>
       </c>
     </row>
@@ -553,28 +569,28 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>140000</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>138000</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>278000</v>
       </c>
     </row>
@@ -582,28 +598,28 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
         <v>55000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>161400</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>216400</v>
       </c>
     </row>
@@ -611,599 +627,755 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2">
-        <v>69300</v>
-      </c>
-      <c r="D5" s="2">
-        <v>120100</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>189400</v>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>100900</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>89000</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>189900</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>169400</v>
-      </c>
-      <c r="D6" s="2">
-        <v>16000</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>185400</v>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>69300</v>
+      </c>
+      <c r="D6">
+        <v>120100</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>189400</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="2">
-        <v>126900</v>
-      </c>
-      <c r="D7" s="2">
-        <v>36900</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <v>163800</v>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>169400</v>
+      </c>
+      <c r="D7">
+        <v>16000</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>185400</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2">
-        <v>136000</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2">
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <v>136000</v>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>126900</v>
+      </c>
+      <c r="D8">
+        <v>36900</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>163800</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
-      </c>
-      <c r="D9" s="2">
-        <v>135000</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <v>135000</v>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>136000</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>136000</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" s="2">
-        <v>133200</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>133200</v>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>135000</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>135000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2">
-        <v>55000</v>
-      </c>
-      <c r="D11" s="2">
-        <v>57800</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>112800</v>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>133200</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>133200</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2">
-        <v>111500</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0</v>
-      </c>
-      <c r="I12" s="2">
-        <v>111500</v>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12">
+        <v>55000</v>
+      </c>
+      <c r="D12">
+        <v>57800</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>112800</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>105400</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>105400</v>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>111500</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>111500</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2">
-        <v>100900</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0</v>
-      </c>
-      <c r="I14" s="2">
-        <v>100900</v>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>102000</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>102000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2">
-        <v>96200</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0</v>
-      </c>
-      <c r="I15" s="2">
-        <v>96200</v>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>99100</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>99100</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>83200</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0</v>
-      </c>
-      <c r="I16" s="2">
-        <v>83200</v>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>96200</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>96200</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="2">
-        <v>81600</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0</v>
-      </c>
-      <c r="I17" s="2">
-        <v>81600</v>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>93100</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>93100</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2">
-        <v>75000</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0</v>
-      </c>
-      <c r="I18" s="2">
-        <v>75000</v>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>83200</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>83200</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2">
-        <v>66400</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0</v>
-      </c>
-      <c r="I19" s="2">
-        <v>66400</v>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>81600</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>81600</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="2">
-        <v>62800</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="2">
-        <v>62800</v>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>75400</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>75400</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2">
-        <v>62000</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0</v>
-      </c>
-      <c r="I21" s="2">
-        <v>62000</v>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>75000</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>75000</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="2">
-        <v>49400</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0</v>
-      </c>
-      <c r="I22" s="2">
-        <v>49400</v>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>71500</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>71500</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="2">
-        <v>28000</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0</v>
-      </c>
-      <c r="I23" s="2">
-        <v>28000</v>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>70700</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>70700</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0</v>
-      </c>
-      <c r="D24" s="2">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24">
+        <v>66400</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>66400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>62800</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>62800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>62000</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>62000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>54200</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>54200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28">
+        <v>49400</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>49400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29">
+        <v>28000</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>25400</v>
       </c>
-      <c r="E24" s="2">
-        <v>0</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0</v>
-      </c>
-      <c r="I24" s="2">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
         <v>25400</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>

</xml_diff>

<commit_message>
Updated leaderboards for week 4
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Downloads\Chrome Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEC227B-ECFF-4042-8EA1-28CA7D613256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B105FA-3531-48AA-B575-5A714EB726D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>#</t>
   </si>
@@ -147,6 +147,33 @@
   </si>
   <si>
     <t>Bervyn Sim</t>
+  </si>
+  <si>
+    <t>Lisa Cheong</t>
+  </si>
+  <si>
+    <t>Jack Sweeney</t>
+  </si>
+  <si>
+    <t>Yongha Kim</t>
+  </si>
+  <si>
+    <t>Kevin Dai</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Ao Fu</t>
+  </si>
+  <si>
+    <t>David Roberts</t>
+  </si>
+  <si>
+    <t>Isabelle Li</t>
+  </si>
+  <si>
+    <t>Vance Lam</t>
   </si>
 </sst>
 </file>
@@ -498,12 +525,12 @@
   <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="27.08984375" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" customWidth="1"/>
     <col min="8" max="8" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -541,19 +568,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>140000</v>
       </c>
       <c r="D2">
-        <v>387500</v>
+        <v>138000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>347200</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -562,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>387500</v>
+        <v>635200</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -570,16 +597,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C3">
-        <v>140000</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>138000</v>
+        <v>387500</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>80300</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -591,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>278000</v>
+        <v>467800</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -599,19 +626,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>55000</v>
+        <v>136000</v>
       </c>
       <c r="D4">
-        <v>161400</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>187000</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>34200</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -620,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>216400</v>
+        <v>357200</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -628,19 +655,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>100900</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>105000</v>
       </c>
       <c r="E5">
-        <v>89000</v>
+        <v>119100</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -649,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>189900</v>
+        <v>349100</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -657,19 +684,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>69300</v>
+        <v>55000</v>
       </c>
       <c r="D6">
-        <v>120100</v>
+        <v>161400</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>85200</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -678,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>189400</v>
+        <v>301600</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -686,19 +713,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>169400</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>16000</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>102000</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>176400</v>
       </c>
       <c r="G7">
         <v>0</v>
@@ -707,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>185400</v>
+        <v>278400</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -715,19 +742,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8">
-        <v>126900</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>36900</v>
+        <v>75400</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>69600</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>125000</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -736,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>163800</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -744,19 +771,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>136000</v>
+        <v>126900</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>36900</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>100000</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -765,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>136000</v>
+        <v>263800</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -773,16 +800,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>135000</v>
+        <v>83200</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>178800</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -794,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>135000</v>
+        <v>262000</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -802,19 +829,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>69300</v>
       </c>
       <c r="D11">
-        <v>133200</v>
+        <v>120100</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>47700</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -823,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>133200</v>
+        <v>237100</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -831,16 +858,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C12">
-        <v>55000</v>
+        <v>114900</v>
       </c>
       <c r="D12">
-        <v>57800</v>
+        <v>50000</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>66800</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -852,7 +879,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>112800</v>
+        <v>231700</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
@@ -860,19 +887,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>100900</v>
       </c>
       <c r="D13">
-        <v>111500</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>89000</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -881,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>111500</v>
+        <v>219900</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -889,19 +916,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>62800</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>102000</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>136100</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -910,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>102000</v>
+        <v>198900</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -918,16 +945,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>169400</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>16000</v>
       </c>
       <c r="E15">
-        <v>99100</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -939,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>99100</v>
+        <v>185400</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -947,19 +974,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="C16">
-        <v>96200</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>88800</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>19100</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>67100</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -968,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>96200</v>
+        <v>175000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -976,16 +1003,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>93100</v>
+        <v>111500</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>63300</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -997,7 +1024,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>93100</v>
+        <v>174800</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1005,19 +1032,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>55000</v>
       </c>
       <c r="D18">
-        <v>83200</v>
+        <v>57800</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>54500</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1026,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>83200</v>
+        <v>172300</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1034,10 +1061,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>81600</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1046,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>149900</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -1055,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>81600</v>
+        <v>149900</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1063,19 +1090,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>75400</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>54200</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>86000</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1084,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>75400</v>
+        <v>140200</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1092,13 +1119,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C21">
-        <v>75000</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>133200</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1113,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>75000</v>
+        <v>133200</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1121,7 +1148,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1130,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>71500</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>130000</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1142,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>71500</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1162,7 +1189,7 @@
         <v>70700</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>56200</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1171,7 +1198,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>70700</v>
+        <v>126900</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
@@ -1179,16 +1206,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C24">
-        <v>66400</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>111800</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -1200,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>66400</v>
+        <v>111800</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
@@ -1208,10 +1235,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C25">
-        <v>62800</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1220,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>101000</v>
       </c>
       <c r="G25">
         <v>0</v>
@@ -1229,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>62800</v>
+        <v>101000</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1237,16 +1264,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C26">
-        <v>62000</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>99100</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1258,7 +1285,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>62000</v>
+        <v>99100</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
@@ -1266,16 +1293,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>96200</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>54200</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1287,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>54200</v>
+        <v>96200</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1295,13 +1322,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C28">
-        <v>49400</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>93100</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1316,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>49400</v>
+        <v>93100</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
@@ -1324,10 +1351,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C29">
-        <v>28000</v>
+        <v>81600</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1345,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>28000</v>
+        <v>81600</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
@@ -1353,82 +1380,316 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>78900</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>78900</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>75000</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>66400</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>66400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>62000</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>62000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34">
+        <v>49400</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>49400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>41500</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>41500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>40500</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>40500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37">
+        <v>28000</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>28000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>29</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-      <c r="D30">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>25400</v>
       </c>
-      <c r="E30">
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-      <c r="I30">
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
         <v>25400</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>21700</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>21700</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
updated poker leaderboard for sem2 r2
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Downloads\code\qts\poker-tournament-leaderboard-2025sem2\poker-tournament-leaderboard\public\res\leaderboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A508DE0D-CFA2-4109-AB66-2A28CCD0A16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D461CEE-8011-4580-B509-502877FE1823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$L$39</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -62,7 +65,115 @@
     <t>Total</t>
   </si>
   <si>
-    <t>-</t>
+    <t>Hansen Wang</t>
+  </si>
+  <si>
+    <t>Siddhanth Jain</t>
+  </si>
+  <si>
+    <t>Charlie Galea</t>
+  </si>
+  <si>
+    <t>Souji Harada</t>
+  </si>
+  <si>
+    <t>Edwin Li</t>
+  </si>
+  <si>
+    <t>Jack Sweeney</t>
+  </si>
+  <si>
+    <t>rachel wang</t>
+  </si>
+  <si>
+    <t>Joshua Kang</t>
+  </si>
+  <si>
+    <t>Isaac Yau</t>
+  </si>
+  <si>
+    <t>Owen Sanigorski</t>
+  </si>
+  <si>
+    <t>Leon Poor</t>
+  </si>
+  <si>
+    <t>Kai Wang</t>
+  </si>
+  <si>
+    <t>The Anh Ngo</t>
+  </si>
+  <si>
+    <t>Max Gao</t>
+  </si>
+  <si>
+    <t>William Nguyen</t>
+  </si>
+  <si>
+    <t>Joshua Burke</t>
+  </si>
+  <si>
+    <t>Abhay Jhade</t>
+  </si>
+  <si>
+    <t>William Yang</t>
+  </si>
+  <si>
+    <t>Yutong Hu</t>
+  </si>
+  <si>
+    <t>Pavan Dev</t>
+  </si>
+  <si>
+    <t>Isabelle Li</t>
+  </si>
+  <si>
+    <t>Benjamin Morrison</t>
+  </si>
+  <si>
+    <t>Murtesa Mohamed Musa</t>
+  </si>
+  <si>
+    <t>Kelven Zhang</t>
+  </si>
+  <si>
+    <t>Daniel Moreno Pintado</t>
+  </si>
+  <si>
+    <t>Benjamin Choi</t>
+  </si>
+  <si>
+    <t>Eric Chang</t>
+  </si>
+  <si>
+    <t>Edwin Zou</t>
+  </si>
+  <si>
+    <t>Andrew Walker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quan </t>
+  </si>
+  <si>
+    <t>Thomas Blanch</t>
+  </si>
+  <si>
+    <t>joel jacobson</t>
+  </si>
+  <si>
+    <t>nick larobine</t>
+  </si>
+  <si>
+    <t>bervyn sim</t>
+  </si>
+  <si>
+    <t>sam narayan</t>
+  </si>
+  <si>
+    <t>charlie wetenhall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ryan Tashiro </t>
   </si>
 </sst>
 </file>
@@ -413,14 +524,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" customWidth="1"/>
+    <col min="9" max="9" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -457,10 +575,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>302100</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -478,7 +596,8 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <f>SUM(C2:H2)</f>
+        <v>302100</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -486,10 +605,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>147800</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -507,7 +626,8 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <f t="shared" ref="I3:I38" si="0">SUM(C3:H3)</f>
+        <v>147800</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -515,10 +635,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>135000</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -536,7 +656,8 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>135000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -544,10 +665,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>109800</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -565,7 +686,8 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>109800</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -573,10 +695,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>109500</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -594,7 +716,8 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>109500</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -602,10 +725,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>100700</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -623,7 +746,8 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>100700</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
@@ -631,10 +755,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>87500</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -652,7 +776,8 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>87500</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -660,10 +785,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>81800</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -681,7 +806,8 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>81800</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -689,142 +815,896 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>80300</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>80300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>78000</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>74800</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>74800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
+      <c r="C13">
+        <v>72800</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>72800</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <v>66100</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>66100</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>63800</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>63800</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>54400</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>54400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>51700</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>51700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>51400</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>51400</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19">
+        <v>51340</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>51340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>50000</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>46600</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>46600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22">
+        <v>46200</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>46200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>43000</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24">
+        <v>40000</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25">
+        <v>37000</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>36100</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>36100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27">
+        <v>35800</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>35800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>35000</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29">
+        <v>33300</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>33300</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>30500</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>30500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>29500</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>29500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32">
+        <v>28800</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>28800</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <v>27400</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34">
+        <v>22200</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>22200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>18200</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>18200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>17100</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>10200</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>3800</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated Leaderboards for R5 Poker
</commit_message>
<xml_diff>
--- a/public/res/leaderboards/Advanced.xlsx
+++ b/public/res/leaderboards/Advanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Downloads\code\qts\poker-tournament-leaderboard-2025sem2\poker-tournament-leaderboard\public\res\leaderboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lh/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FA75A4-ABCB-4C9D-9648-8D35147736B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDFE900-A8A5-F34C-9141-4F6B2BC7719F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4180" yWindow="3100" windowWidth="30240" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$K$1:$L$39</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>#</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Jamie Kukuruzovic</t>
   </si>
   <si>
-    <t>Achal Jhawar</t>
-  </si>
-  <si>
     <t>Gordon Wu</t>
   </si>
   <si>
@@ -236,30 +233,18 @@
     <t>Tony Liu</t>
   </si>
   <si>
-    <t>Beginner</t>
-  </si>
-  <si>
     <t>Arihant Rawal</t>
   </si>
   <si>
     <t>Jay Timothy Wang</t>
   </si>
   <si>
-    <t>Natty Ayano</t>
-  </si>
-  <si>
-    <t>Ryan Kin</t>
-  </si>
-  <si>
     <t>Shakhruz Rakhmatullaev</t>
   </si>
   <si>
     <t>Akash Jayaprabalan</t>
   </si>
   <si>
-    <t>Sparsh Basantani</t>
-  </si>
-  <si>
     <t>Tianhong Deng</t>
   </si>
   <si>
@@ -267,6 +252,9 @@
   </si>
   <si>
     <t>Mohit Garg</t>
+  </si>
+  <si>
+    <t>Zarif Syed</t>
   </si>
 </sst>
 </file>
@@ -617,24 +605,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="10.90625" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -663,24 +651,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>302100</v>
+        <v>80300</v>
       </c>
       <c r="D2">
-        <v>53700</v>
+        <v>9000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>180000</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>109000</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -689,21 +677,21 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>355800</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>378300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>30500</v>
+        <v>302100</v>
       </c>
       <c r="D3">
-        <v>298500</v>
+        <v>53700</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -718,21 +706,21 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>314000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>355800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>30500</v>
       </c>
       <c r="D4">
-        <v>298700</v>
+        <v>298500</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -747,27 +735,27 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>298700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>314000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C5">
-        <v>109500</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>168700</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>200000</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>112000</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -776,27 +764,27 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>278200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>312000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>80300</v>
+        <v>109500</v>
       </c>
       <c r="D6">
-        <v>9000</v>
+        <v>168700</v>
       </c>
       <c r="E6">
-        <v>180000</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -805,21 +793,21 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>269300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>303200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C7">
-        <v>74800</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>156000</v>
+        <v>298700</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -834,27 +822,27 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>215800</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>298700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>52000</v>
       </c>
       <c r="E8">
-        <v>200000</v>
+        <v>120700</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>103500</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -863,27 +851,27 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>276200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>87500</v>
       </c>
       <c r="D9">
-        <v>52000</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>120700</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>181200</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -892,27 +880,27 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>172700</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>268700</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10">
-        <v>109800</v>
+        <v>100700</v>
       </c>
       <c r="D10">
-        <v>61100</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>163000</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -921,27 +909,27 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>170900</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>263700</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="C11">
-        <v>120000</v>
+        <v>64500</v>
       </c>
       <c r="D11">
-        <v>16200</v>
+        <v>22500</v>
       </c>
       <c r="E11">
-        <v>24500</v>
+        <v>54100</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>98100</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -950,21 +938,21 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>160700</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+        <v>224200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>71000</v>
+        <v>74800</v>
       </c>
       <c r="D12">
-        <v>81400</v>
+        <v>156000</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -979,21 +967,21 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>152400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+        <v>215800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>147800</v>
+        <v>109800</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>61100</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1008,27 +996,27 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>147800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>170900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>89800</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>54100</v>
+        <v>44000</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>140000</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1037,24 +1025,24 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>143900</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>169000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>64500</v>
+        <v>120000</v>
       </c>
       <c r="D15">
-        <v>37500</v>
+        <v>16200</v>
       </c>
       <c r="E15">
-        <v>54100</v>
+        <v>24500</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1066,27 +1054,27 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>126100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>160700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>51340</v>
+        <v>18200</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>37000</v>
       </c>
       <c r="E16">
-        <v>72000</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1095,24 +1083,24 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>123340</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>160200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17">
-        <v>27400</v>
+        <v>147800</v>
       </c>
       <c r="D17">
-        <v>48000</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>35300</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1124,24 +1112,24 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>110700</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>147800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C18">
-        <v>100700</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>89800</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>54100</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1153,24 +1141,24 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>100700</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>143900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>51340</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>95800</v>
+        <v>72000</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1182,24 +1170,24 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>95800</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>123340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>89300</v>
+        <v>27400</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>48000</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>35300</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1211,24 +1199,24 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>89300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>110700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>87500</v>
+        <v>10200</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>97900</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -1240,24 +1228,24 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>87500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>108100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>83600</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>95800</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -1269,18 +1257,18 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>83600</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>95800</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C23">
-        <v>81800</v>
+        <v>89300</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1298,27 +1286,27 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>81800</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>89300</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C24">
-        <v>17100</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>63500</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>22000</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>62400</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1327,24 +1315,24 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>80600</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>84400</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>83600</v>
       </c>
       <c r="E25">
-        <v>78000</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1356,18 +1344,18 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>83600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C26">
-        <v>78000</v>
+        <v>81800</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1385,21 +1373,21 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>81800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C27">
-        <v>72800</v>
+        <v>17100</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>63500</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1414,21 +1402,21 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>72800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>80600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>78000</v>
       </c>
       <c r="D28">
-        <v>72000</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1443,18 +1431,18 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <v>72000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>66100</v>
+        <v>72800</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1472,21 +1460,21 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>66100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72800</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>64800</v>
+        <v>72000</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1501,18 +1489,18 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <v>64800</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C31">
-        <v>63800</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1521,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>85400</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1530,27 +1518,27 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <v>63800</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>70400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>55500</v>
+        <v>28000</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>41000</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -1559,18 +1547,18 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <v>55500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>69000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C33">
-        <v>54400</v>
+        <v>66100</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1588,21 +1576,21 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <v>54400</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>66100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>63800</v>
       </c>
       <c r="D34">
-        <v>54000</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1617,27 +1605,27 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>54000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>63800</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C35">
-        <v>51700</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>33000</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>28300</v>
       </c>
       <c r="G35">
         <v>0</v>
@@ -1646,27 +1634,27 @@
         <v>0</v>
       </c>
       <c r="I35">
-        <v>51700</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>61300</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C36">
-        <v>51400</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>28500</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>30900</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -1675,24 +1663,24 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <v>51400</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>59400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>32500</v>
+        <v>55500</v>
       </c>
       <c r="E37">
-        <v>32500</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -1704,18 +1692,18 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>55500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C38">
-        <v>50000</v>
+        <v>54400</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1733,24 +1721,24 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>54400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>51700</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>49800</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1762,21 +1750,21 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <v>49800</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>51700</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>51400</v>
       </c>
       <c r="D40">
-        <v>49300</v>
+        <v>0</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -1791,18 +1779,18 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <v>49300</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+        <v>51400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C41">
-        <v>46600</v>
+        <v>50000</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1820,24 +1808,24 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <v>46600</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C42">
-        <v>46200</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>49800</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -1849,24 +1837,24 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>46200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>49300</v>
       </c>
       <c r="E43">
-        <v>44000</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -1878,21 +1866,21 @@
         <v>0</v>
       </c>
       <c r="I43">
-        <v>44000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>46600</v>
       </c>
       <c r="D44">
-        <v>43400</v>
+        <v>0</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -1907,18 +1895,18 @@
         <v>0</v>
       </c>
       <c r="I44">
-        <v>43400</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C45">
-        <v>43000</v>
+        <v>46200</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1936,24 +1924,24 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <v>43000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+        <v>46200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="C46">
-        <v>18200</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>37000</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>44000</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -1965,21 +1953,21 @@
         <v>0</v>
       </c>
       <c r="I46">
-        <v>40200</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+        <v>44000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C47">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>43400</v>
       </c>
       <c r="E47">
         <v>0</v>
@@ -1994,21 +1982,21 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+        <v>43400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>43000</v>
       </c>
       <c r="D48">
-        <v>38900</v>
+        <v>0</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2023,24 +2011,24 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <v>38900</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+        <v>43000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>73</v>
+        <v>36</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>37500</v>
+        <v>0</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -2052,21 +2040,21 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <v>37500</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C50">
-        <v>37000</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>54000</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2081,21 +2069,21 @@
         <v>0</v>
       </c>
       <c r="I50">
-        <v>37000</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+        <v>39000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C51">
-        <v>36100</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>38900</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2110,18 +2098,18 @@
         <v>0</v>
       </c>
       <c r="I51">
-        <v>36100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>38900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="C52">
-        <v>35800</v>
+        <v>37000</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2139,21 +2127,21 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>35800</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>36100</v>
       </c>
       <c r="D53">
-        <v>35500</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2168,18 +2156,18 @@
         <v>0</v>
       </c>
       <c r="I53">
-        <v>35500</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+        <v>36100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C54">
-        <v>35000</v>
+        <v>35800</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -2197,21 +2185,21 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+        <v>35800</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="C55">
-        <v>33300</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>35500</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2226,21 +2214,21 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <v>33300</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+        <v>35500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>35000</v>
       </c>
       <c r="D56">
-        <v>33000</v>
+        <v>0</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2255,24 +2243,24 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <v>33000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>33300</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="E57">
-        <v>44000</v>
+        <v>0</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -2284,10 +2272,10 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <v>29000</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2316,21 +2304,21 @@
         <v>28800</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>28500</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>25400</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2342,10 +2330,10 @@
         <v>0</v>
       </c>
       <c r="I59">
-        <v>28500</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+        <v>25400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2356,7 +2344,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>28000</v>
+        <v>25000</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -2371,24 +2359,24 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <v>28000</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>22200</v>
       </c>
       <c r="D61">
         <v>0</v>
       </c>
       <c r="E61">
-        <v>25400</v>
+        <v>0</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -2400,21 +2388,21 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <v>25400</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+        <v>22200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>14500</v>
       </c>
       <c r="D62">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2429,21 +2417,21 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+        <v>14500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="C63">
-        <v>22200</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>13500</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2458,24 +2446,24 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <v>22200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>3800</v>
       </c>
       <c r="D64">
         <v>0</v>
       </c>
       <c r="E64">
-        <v>22000</v>
+        <v>0</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -2487,10 +2475,10 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2519,12 +2507,12 @@
         <v>14500</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2548,7 +2536,7 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2577,12 +2565,12 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2606,7 +2594,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2635,184 +2623,184 @@
         <v>3800</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
     </row>
   </sheetData>

</xml_diff>